<commit_message>
july 5 delivery update
</commit_message>
<xml_diff>
--- a/recommendations.xlsx
+++ b/recommendations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaspetitjean/Dropbox/work/call-it-spring/deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4796C0-5852-8946-A21F-6F8EAF3FC338}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78896EDE-DB5A-F249-908A-F59A0B8E1AC3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="21160" xr2:uid="{05FB31AA-17C6-1542-BE25-C36D348B0708}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="80">
   <si>
     <t>Priority level</t>
   </si>
@@ -74,231 +74,205 @@
     <t>Product Urls (colours)</t>
   </si>
   <si>
-    <t>Recommendation</t>
-  </si>
-  <si>
     <t>Product availability</t>
   </si>
   <si>
-    <t>What will be the server status code on temporarily unavailable products?
-What will be the server status code on discontinued products (redirections)?</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
+    <t>Global banner</t>
+  </si>
+  <si>
+    <t>PDP 5 angles TBC</t>
+  </si>
+  <si>
+    <t>P00-Homepage</t>
+  </si>
+  <si>
+    <t>P01-Gender_Landing</t>
+  </si>
+  <si>
+    <t>P02-PLP</t>
+  </si>
+  <si>
+    <t>P03-PLP_Deluxe</t>
+  </si>
+  <si>
+    <t>P04-PLP_Sales</t>
+  </si>
+  <si>
+    <t>P05-Me_to_We</t>
+  </si>
+  <si>
+    <t>P06-Trend</t>
+  </si>
+  <si>
+    <t>P07-Instashop</t>
+  </si>
+  <si>
+    <t>P08-Wishlist</t>
+  </si>
+  <si>
+    <t>P09-PDP</t>
+  </si>
+  <si>
+    <t>P10-Gift_Card</t>
+  </si>
+  <si>
+    <t>P11-Checkout</t>
+  </si>
+  <si>
+    <t>P12-Account</t>
+  </si>
+  <si>
+    <t>P13-404</t>
+  </si>
+  <si>
+    <t>P14-Legal</t>
+  </si>
+  <si>
+    <t>P15-International</t>
+  </si>
+  <si>
+    <t>X00 - Styleguide</t>
+  </si>
+  <si>
+    <t>X01-Footer</t>
+  </si>
+  <si>
+    <t>X02-Cookie</t>
+  </si>
+  <si>
+    <t>X03-Modal_Account_Sign_In</t>
+  </si>
+  <si>
+    <t>X04-Modal_Error</t>
+  </si>
+  <si>
+    <t>X05-Size_Guide</t>
+  </si>
+  <si>
+    <t>X06-Search</t>
+  </si>
+  <si>
+    <t>X07-Navigation</t>
+  </si>
+  <si>
+    <t>X08-Filter</t>
+  </si>
+  <si>
+    <t>X09-Store_Locator</t>
+  </si>
+  <si>
+    <t>X10-Promos</t>
+  </si>
+  <si>
+    <t>T01-VOC</t>
+  </si>
+  <si>
+    <t>T02-True_Fit</t>
+  </si>
+  <si>
+    <t>T03-Live_Chat</t>
+  </si>
+  <si>
+    <t>Components &amp; Pages</t>
+  </si>
+  <si>
+    <t>SEO Benefit</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Hreflang</t>
+  </si>
+  <si>
+    <t>UX-related</t>
+  </si>
+  <si>
+    <t>Breadcrumbs - Product Pages</t>
+  </si>
+  <si>
+    <t>Sitemap images</t>
+  </si>
+  <si>
+    <t>PageSpeed</t>
+  </si>
+  <si>
+    <t>Linking</t>
+  </si>
+  <si>
+    <t>Open graph</t>
+  </si>
+  <si>
+    <t>Store locator</t>
+  </si>
+  <si>
+    <t>Implement hreflang tags on each page or add an hreflang sitemap, whatever is easiest.</t>
+  </si>
+  <si>
+    <t>Sitemap index</t>
+  </si>
+  <si>
+    <t>Sitemap pages</t>
+  </si>
+  <si>
+    <t>On product pages: add a link to the homepage in position 1.</t>
+  </si>
+  <si>
+    <t>Recommendations</t>
+  </si>
+  <si>
+    <t>Waiting for MVP (July 17).</t>
+  </si>
+  <si>
+    <t>See /hreflang/hreflang-tags.md or /hreflang/sitemap-hreflang.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+See pagination.md</t>
+  </si>
+  <si>
+    <t>Request for better crawling and for browsers with JavaScript disabled: add links to the rest of the paginated pages at the bottom of every paginated page.</t>
+  </si>
+  <si>
+    <t>See links.md</t>
+  </si>
+  <si>
+    <t>Have one, non-colour specific, URL per product.
+Load the colours in the same page, using JS to lazy load the other product images.</t>
+  </si>
+  <si>
+    <t>See open-graph.md</t>
+  </si>
+  <si>
+    <t>See sitemap-index.xml</t>
+  </si>
+  <si>
+    <t>See sitemap-pages.xml</t>
+  </si>
+  <si>
+    <t>See sitemap-images.xml</t>
+  </si>
+  <si>
+    <t>See structured-data.md</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
     <t>Leave the product page as is for temporarily unavailable products.
-Redirect discontinued product pages to the most relevant category/PDP.</t>
-  </si>
-  <si>
-    <t>Global banner</t>
-  </si>
-  <si>
-    <t>PDP 5 angles TBC</t>
-  </si>
-  <si>
-    <t>P00-Homepage</t>
-  </si>
-  <si>
-    <t>P01-Gender_Landing</t>
-  </si>
-  <si>
-    <t>P02-PLP</t>
-  </si>
-  <si>
-    <t>P03-PLP_Deluxe</t>
-  </si>
-  <si>
-    <t>P04-PLP_Sales</t>
-  </si>
-  <si>
-    <t>P05-Me_to_We</t>
-  </si>
-  <si>
-    <t>P06-Trend</t>
-  </si>
-  <si>
-    <t>P07-Instashop</t>
-  </si>
-  <si>
-    <t>P08-Wishlist</t>
-  </si>
-  <si>
-    <t>P09-PDP</t>
-  </si>
-  <si>
-    <t>P10-Gift_Card</t>
-  </si>
-  <si>
-    <t>P11-Checkout</t>
-  </si>
-  <si>
-    <t>P12-Account</t>
-  </si>
-  <si>
-    <t>P13-404</t>
-  </si>
-  <si>
-    <t>P14-Legal</t>
-  </si>
-  <si>
-    <t>P15-International</t>
-  </si>
-  <si>
-    <t>X00 - Styleguide</t>
-  </si>
-  <si>
-    <t>X01-Footer</t>
-  </si>
-  <si>
-    <t>X02-Cookie</t>
-  </si>
-  <si>
-    <t>X03-Modal_Account_Sign_In</t>
-  </si>
-  <si>
-    <t>X04-Modal_Error</t>
-  </si>
-  <si>
-    <t>X05-Size_Guide</t>
-  </si>
-  <si>
-    <t>X06-Search</t>
-  </si>
-  <si>
-    <t>X07-Navigation</t>
-  </si>
-  <si>
-    <t>X08-Filter</t>
-  </si>
-  <si>
-    <t>X09-Store_Locator</t>
-  </si>
-  <si>
-    <t>X10-Promos</t>
-  </si>
-  <si>
-    <t>T01-VOC</t>
-  </si>
-  <si>
-    <t>T02-True_Fit</t>
-  </si>
-  <si>
-    <t>T03-Live_Chat</t>
-  </si>
-  <si>
-    <t>Components &amp; Pages</t>
-  </si>
-  <si>
-    <t>SEO Benefit</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Hreflang</t>
-  </si>
-  <si>
-    <t>UX-related</t>
-  </si>
-  <si>
-    <t>Breadcrumbs - Product Pages</t>
-  </si>
-  <si>
-    <t>Infinite scroll</t>
-  </si>
-  <si>
-    <t>Standby.</t>
-  </si>
-  <si>
-    <t>Sitemap images</t>
-  </si>
-  <si>
-    <t>Search Console setup</t>
-  </si>
-  <si>
-    <t>Verify media subdomain on Search Console.
-Add http &amp; https versions of the domains</t>
-  </si>
-  <si>
-    <t>Image Optimization</t>
-  </si>
-  <si>
-    <t>Add alt attribute on product images.</t>
-  </si>
-  <si>
-    <t>PageSpeed</t>
-  </si>
-  <si>
-    <t>Linking</t>
-  </si>
-  <si>
-    <t>In Progress.</t>
-  </si>
-  <si>
-    <t>Open graph</t>
-  </si>
-  <si>
-    <t>Store locator</t>
-  </si>
-  <si>
-    <t>See open-graph.html</t>
-  </si>
-  <si>
-    <t>See robots.txt</t>
-  </si>
-  <si>
-    <t>Implement hreflang tags on each page or add an hreflang sitemap, whatever is easiest.</t>
-  </si>
-  <si>
-    <t>See /hreflang/hreflang-tags.html or /hreflang/sitemap-hreflang.xml</t>
-  </si>
-  <si>
-    <t>See pagination.html</t>
-  </si>
-  <si>
-    <t>See links.html</t>
-  </si>
-  <si>
-    <t>Have one, non-colour specific, URL per product.
-Load the colours in the same page, using JS to lazy Load the other product images.</t>
-  </si>
-  <si>
-    <t>In progress.</t>
-  </si>
-  <si>
-    <t>Sitemap index</t>
-  </si>
-  <si>
-    <t>See sitemap-index.html</t>
-  </si>
-  <si>
-    <t>See sitemap-pages.html</t>
-  </si>
-  <si>
-    <t>See sitemap-images.html</t>
-  </si>
-  <si>
-    <t>Sitemap pages</t>
-  </si>
-  <si>
-    <t>See structured-data.html</t>
-  </si>
-  <si>
-    <t>On product pages: add a link to the homepage in position 1.</t>
-  </si>
-  <si>
-    <t>See performance.html
-Deliver site assets (product images, hero/content images and navigation icons) through a content delivery network and set a server caching rule. Media cache should be busted when assets are modified.</t>
-  </si>
-  <si>
-    <t>None.</t>
+Redirect discontinued product pages to the most relevant category / landing / list page.</t>
+  </si>
+  <si>
+    <t>Please confirm that price can be displayed in the SERP considering that CIS' sale periods. See comments in product markup.</t>
   </si>
 </sst>
 </file>
@@ -486,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -547,6 +521,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -904,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC96CD3-FCC3-3149-BCBA-07675048BF3E}">
-  <dimension ref="A2:F30"/>
+  <dimension ref="A2:F28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -960,10 +943,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>0</v>
@@ -985,11 +968,9 @@
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>10</v>
@@ -999,13 +980,13 @@
     </row>
     <row r="10" spans="1:6" ht="30">
       <c r="A10" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>9</v>
@@ -1013,15 +994,15 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="19">
+    <row r="11" spans="1:6" ht="45">
       <c r="A11" s="6" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>10</v>
@@ -1029,128 +1010,116 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="19">
       <c r="A12" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>87</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="19">
-      <c r="A13" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="19">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
+      <c r="A14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="19">
-      <c r="A15" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
+    <row r="15" spans="1:6" ht="45">
+      <c r="A15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="45">
-      <c r="A16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="A16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="26" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="19">
       <c r="A17" s="6" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>16</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="19">
       <c r="A18" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>65</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" ht="19">
       <c r="A19" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>78</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" ht="19">
       <c r="A20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="7"/>
       <c r="D20" s="8" t="s">
         <v>10</v>
       </c>
@@ -1159,14 +1128,12 @@
     </row>
     <row r="21" spans="1:6" ht="19">
       <c r="A21" s="6" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>78</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
         <v>10</v>
       </c>
@@ -1174,112 +1141,76 @@
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" ht="19">
-      <c r="A22" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" ht="19">
-      <c r="A23" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="A23" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" ht="19">
-      <c r="A24" s="3"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="3"/>
+    <row r="24" spans="1:6" ht="30">
+      <c r="A24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" ht="19">
-      <c r="A25" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
     <row r="26" spans="1:6" ht="19">
-      <c r="A26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="A26" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
+    <row r="27" spans="1:6" ht="19">
+      <c r="A27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
     <row r="28" spans="1:6" ht="19">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" ht="19">
-      <c r="A29" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" ht="60">
-      <c r="A30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1292,7 +1223,7 @@
           <x14:formula1>
             <xm:f>data!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D26 D9:D13 D29:D30 D16:D23</xm:sqref>
+          <xm:sqref>D24 D27:D28 D9:D12 D15:D21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1316,269 +1247,269 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="23" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>